<commit_message>
[Feat 2269] moar debug
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/call-steps.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/call-steps.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="13560" windowHeight="5076"/>
   </bookViews>
   <sheets>
     <sheet name="STEPS" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -61,20 +62,20 @@
     <t>1</t>
   </si>
   <si>
-    <t>call/path/1</t>
-  </si>
-  <si>
-    <t>call/path/2</t>
-  </si>
-  <si>
-    <t>call/path/3</t>
+    <t>CALL /path/1</t>
+  </si>
+  <si>
+    <t>CALL /path/2</t>
+  </si>
+  <si>
+    <t>CALL /path/3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -255,7 +255,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,29 +430,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -488,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -507,7 +506,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -526,7 +525,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>13</v>

</xml_diff>